<commit_message>
minor updates after meeting
</commit_message>
<xml_diff>
--- a/EC/Train Runs and Enforcements 2016-06-25.xlsx
+++ b/EC/Train Runs and Enforcements 2016-06-25.xlsx
@@ -2143,125 +2143,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal_XINGS" xfId="1"/>
   </cellStyles>
-  <dxfs count="19">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="9">
     <dxf>
       <font>
         <color rgb="FF9C6500"/>
@@ -2307,6 +2189,36 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2592,8 +2504,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CM166"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A40" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="R63" sqref="R63"/>
+    <sheetView showGridLines="0" topLeftCell="A55" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="R79" sqref="R79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11735,11 +11647,11 @@
         <v>1</v>
       </c>
       <c r="Y102" s="48">
-        <f t="shared" ref="Y102:Y123" si="58">RIGHT(D102,LEN(D102)-4)/10000</f>
+        <f t="shared" ref="Y102:Y117" si="58">RIGHT(D102,LEN(D102)-4)/10000</f>
         <v>4.8000000000000001E-2</v>
       </c>
       <c r="Z102" s="48">
-        <f t="shared" ref="Z102:Z123" si="59">RIGHT(H102,LEN(H102)-4)/10000</f>
+        <f t="shared" ref="Z102:Z117" si="59">RIGHT(H102,LEN(H102)-4)/10000</f>
         <v>23.330500000000001</v>
       </c>
       <c r="AA102" s="48">
@@ -14418,7 +14330,7 @@
         <v>https://search-rtdc-monitor-bjffxe2xuh6vdkpspy63sjmuny.us-east-1.es.amazonaws.com/_plugin/kibana/#/discover/Steve-Slow-Train-Analysis-(2080s-and-2083s)?_g=(refreshInterval:(display:Off,section:0,value:0),time:(from:'2016-06-25 18:25:48-0600',mode:absolute,to:'2016-06-25 19:18:49-0600'))&amp;_a=(columns:!(Source,'Data.Head%20End%20Milepost',Data.Speed,'Data.Locomotive%20State','Data.Train%20ID','Data.Warning%2FEnforcement%20Type','Data.Target%20Start%20Milepost','Data.Target%20Description','Data.Target%20Speed','Data.Enforcement%20Train%20Speed','Data.Enforcement%20Start%20Milepost','Data.Target%20Type','Data.Enforcement%20Direction%20of%20Travel','Message%20ID','Data.Body%20of%20Summary%20Text'),filters:!(),index:'emp_*',interval:auto,query:(query_string:(analyze_wildcard:!t,query:'Message%5C%20ID:(2083%20OR%202080%20OR%201041)%20AND%20%22rtdc.l.rtdc.4027%22')),sort:!(Time,asc))</v>
       </c>
       <c r="W130" s="48" t="str">
-        <f t="shared" ref="W124:W131" si="74">IF(AA130&lt;23,"Y","N")</f>
+        <f t="shared" ref="W130:W131" si="74">IF(AA130&lt;23,"Y","N")</f>
         <v>N</v>
       </c>
       <c r="X130" s="48">
@@ -14426,15 +14338,15 @@
         <v>1</v>
       </c>
       <c r="Y130" s="48">
-        <f t="shared" ref="Y124:Y131" si="75">RIGHT(D130,LEN(D130)-4)/10000</f>
+        <f t="shared" ref="Y130:Y131" si="75">RIGHT(D130,LEN(D130)-4)/10000</f>
         <v>4.5699999999999998E-2</v>
       </c>
       <c r="Z130" s="48">
-        <f t="shared" ref="Z124:Z131" si="76">RIGHT(H130,LEN(H130)-4)/10000</f>
+        <f t="shared" ref="Z130:Z131" si="76">RIGHT(H130,LEN(H130)-4)/10000</f>
         <v>23.331099999999999</v>
       </c>
       <c r="AA130" s="48">
-        <f t="shared" ref="AA124:AA131" si="77">ABS(Z130-Y130)</f>
+        <f t="shared" ref="AA130:AA131" si="77">ABS(Z130-Y130)</f>
         <v>23.285399999999999</v>
       </c>
       <c r="AB130" s="49" t="e">
@@ -17019,27 +16931,27 @@
     <mergeCell ref="I3:J3"/>
   </mergeCells>
   <conditionalFormatting sqref="W11:W12 W13:X1048576">
-    <cfRule type="cellIs" dxfId="12" priority="69" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="69" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X13:X1048576">
-    <cfRule type="cellIs" dxfId="11" priority="52" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="7" priority="52" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X12:X1048576">
-    <cfRule type="cellIs" dxfId="10" priority="49" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="49" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B135:M135 A13:S13 S13:S29 A136:M143 A144:S156 A14:M134 N117:R156 N14:S143">
-    <cfRule type="expression" dxfId="18" priority="45">
+    <cfRule type="expression" dxfId="5" priority="45">
       <formula>$O13&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A13:S156">
-    <cfRule type="expression" dxfId="17" priority="44">
+    <cfRule type="expression" dxfId="4" priority="44">
       <formula>$P13&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17071,8 +16983,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q81"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="N59" sqref="N59"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="N14" sqref="N14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20520,17 +20432,17 @@
     <mergeCell ref="A5:M5"/>
   </mergeCells>
   <conditionalFormatting sqref="P6 M6:N6 M7:M1048576">
-    <cfRule type="cellIs" dxfId="15" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="10" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A7:N81">
-    <cfRule type="expression" dxfId="14" priority="3">
+    <cfRule type="expression" dxfId="1" priority="3">
       <formula>$M7="Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M2:M3">
-    <cfRule type="cellIs" dxfId="13" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>